<commit_message>
test sheet adopted default sleep added
</commit_message>
<xml_diff>
--- a/dLiveChannelListTesting.xlsx
+++ b/dLiveChannelListTesting.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="207">
   <si>
     <t xml:space="preserve">Channel</t>
   </si>
@@ -147,7 +147,7 @@
     <t xml:space="preserve">Mute8</t>
   </si>
   <si>
-    <t xml:space="preserve">KickIn</t>
+    <t xml:space="preserve">TST001</t>
   </si>
   <si>
     <t xml:space="preserve">blue</t>
@@ -162,163 +162,406 @@
     <t xml:space="preserve">x</t>
   </si>
   <si>
-    <t xml:space="preserve">KickOut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SnTop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SnBot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rack1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rack2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Floor1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Floor2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ride</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OH L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OH R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cajon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">empty</t>
+    <t xml:space="preserve">TST002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST014</t>
   </si>
   <si>
     <t xml:space="preserve">black</t>
   </si>
   <si>
-    <t xml:space="preserve">emtpy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BassDI</t>
+    <t xml:space="preserve">TST015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST017</t>
   </si>
   <si>
     <t xml:space="preserve">red</t>
   </si>
   <si>
-    <t xml:space="preserve">BassMi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EGit1L</t>
+    <t xml:space="preserve">TST018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST019</t>
   </si>
   <si>
     <t xml:space="preserve">yellow</t>
   </si>
   <si>
-    <t xml:space="preserve">EGit1R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EGit2L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EGit2R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EGit3L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EGit3R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accu1L</t>
+    <t xml:space="preserve">TST020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST025</t>
   </si>
   <si>
     <t xml:space="preserve">green</t>
   </si>
   <si>
-    <t xml:space="preserve">Accu1R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accu2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accu3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Key1L</t>
+    <t xml:space="preserve">TST026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST029</t>
   </si>
   <si>
     <t xml:space="preserve">light blue</t>
   </si>
   <si>
-    <t xml:space="preserve">Key1R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Key2L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Key2R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Key3L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Key3R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Key4L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Key4R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Divrs1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Divrs2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Divrs3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Divrs4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lead1</t>
+    <t xml:space="preserve">TST030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST032</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST036</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST037</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST038</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST039</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST040</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST041</t>
   </si>
   <si>
     <t xml:space="preserve">white</t>
   </si>
   <si>
-    <t xml:space="preserve">Lead2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lead3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lead4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BV1</t>
+    <t xml:space="preserve">TST042</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST043</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST044</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST045</t>
   </si>
   <si>
     <t xml:space="preserve">purple</t>
   </si>
   <si>
-    <t xml:space="preserve">BV2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BV3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BV4</t>
+    <t xml:space="preserve">TST046</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST047</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST048</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST051</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST052</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST053</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST054</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST055</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST056</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST057</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST058</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST059</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST060</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST061</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST062</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST063</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST064</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST065</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST066</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST067</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST068</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST069</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST070</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST071</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST072</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST073</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST074</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST075</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST076</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST077</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST078</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST079</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST080</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST081</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST082</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST083</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST084</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST085</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST086</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST087</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST088</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST089</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST090</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST091</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST092</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST093</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST094</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST095</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST096</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST097</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST098</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST099</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST104</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST106</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST108</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST109</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST113</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST114</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST116</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST117</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST118</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST119</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST121</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST122</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST124</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST127</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST128</t>
   </si>
   <si>
     <t xml:space="preserve">Indication Start/End Channel
@@ -700,8 +943,8 @@
   </sheetPr>
   <dimension ref="A1:XFD131"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A114" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E130" activeCellId="0" sqref="E130:E131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1361,7 +1604,7 @@
       <c r="A15" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="6" t="s">
         <v>58</v>
       </c>
       <c r="C15" s="7" t="s">
@@ -1371,7 +1614,7 @@
         <v>44</v>
       </c>
       <c r="E15" s="7" t="n">
-        <v>-99</v>
+        <v>10</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>43</v>
@@ -1403,7 +1646,7 @@
         <v>43</v>
       </c>
       <c r="E16" s="7" t="n">
-        <v>-99</v>
+        <v>5</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>44</v>
@@ -1426,7 +1669,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>59</v>
@@ -1435,7 +1678,7 @@
         <v>44</v>
       </c>
       <c r="E17" s="7" t="n">
-        <v>-99</v>
+        <v>0</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>43</v>
@@ -1458,16 +1701,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E18" s="7" t="n">
-        <v>-99</v>
+        <v>-5</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>44</v>
@@ -1493,16 +1736,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>62</v>
-      </c>
       <c r="D19" s="2" t="s">
         <v>44</v>
       </c>
       <c r="E19" s="7" t="n">
-        <v>-99</v>
+        <v>-10</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>43</v>
@@ -1528,16 +1771,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="7" t="n">
-        <v>-99</v>
+        <v>-15</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>44</v>
@@ -1563,16 +1806,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>65</v>
-      </c>
       <c r="D21" s="2" t="s">
         <v>44</v>
       </c>
       <c r="E21" s="7" t="n">
-        <v>-99</v>
+        <v>-20</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>43</v>
@@ -1598,16 +1841,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E22" s="7" t="n">
-        <v>-99</v>
+        <v>-25</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>44</v>
@@ -1633,16 +1876,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>44</v>
       </c>
       <c r="E23" s="7" t="n">
-        <v>-99</v>
+        <v>-30</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>43</v>
@@ -1668,16 +1911,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E24" s="7" t="n">
-        <v>-99</v>
+        <v>-35</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>44</v>
@@ -1703,16 +1946,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>44</v>
       </c>
       <c r="E25" s="7" t="n">
-        <v>-99</v>
+        <v>-40</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>43</v>
@@ -1738,16 +1981,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E26" s="7" t="n">
-        <v>-99</v>
+        <v>-45</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>44</v>
@@ -1773,10 +2016,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>72</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>44</v>
@@ -1808,16 +2051,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E28" s="7" t="n">
-        <v>-99</v>
+        <v>10</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>44</v>
@@ -1843,16 +2086,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>44</v>
       </c>
       <c r="E29" s="7" t="n">
-        <v>-99</v>
+        <v>5</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>43</v>
@@ -1878,16 +2121,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E30" s="7" t="n">
-        <v>-99</v>
+        <v>0</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>44</v>
@@ -1913,16 +2156,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C31" s="7" t="s">
-        <v>77</v>
-      </c>
       <c r="D31" s="2" t="s">
         <v>44</v>
       </c>
       <c r="E31" s="7" t="n">
-        <v>-99</v>
+        <v>-5</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>43</v>
@@ -1948,16 +2191,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E32" s="7" t="n">
-        <v>-99</v>
+        <v>-10</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>44</v>
@@ -1983,16 +2226,16 @@
         <v>32</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>44</v>
       </c>
       <c r="E33" s="7" t="n">
-        <v>-99</v>
+        <v>-15</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>43</v>
@@ -2018,16 +2261,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E34" s="7" t="n">
-        <v>-99</v>
+        <v>-20</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>44</v>
@@ -2053,16 +2296,16 @@
         <v>34</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>44</v>
       </c>
       <c r="E35" s="7" t="n">
-        <v>-99</v>
+        <v>-25</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>43</v>
@@ -2088,16 +2331,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E36" s="7" t="n">
-        <v>-99</v>
+        <v>-30</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>44</v>
@@ -2123,16 +2366,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>44</v>
       </c>
       <c r="E37" s="7" t="n">
-        <v>-99</v>
+        <v>-35</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>43</v>
@@ -2158,7 +2401,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>59</v>
@@ -2167,7 +2410,7 @@
         <v>43</v>
       </c>
       <c r="E38" s="7" t="n">
-        <v>-99</v>
+        <v>-40</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>44</v>
@@ -2193,7 +2436,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>59</v>
@@ -2202,7 +2445,7 @@
         <v>44</v>
       </c>
       <c r="E39" s="7" t="n">
-        <v>-99</v>
+        <v>-45</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>43</v>
@@ -2228,7 +2471,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>59</v>
@@ -2263,7 +2506,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>59</v>
@@ -2272,7 +2515,7 @@
         <v>44</v>
       </c>
       <c r="E41" s="7" t="n">
-        <v>-99</v>
+        <v>10</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>43</v>
@@ -2298,16 +2541,16 @@
         <v>41</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E42" s="7" t="n">
-        <v>-99</v>
+        <v>5</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>44</v>
@@ -2333,16 +2576,16 @@
         <v>42</v>
       </c>
       <c r="B43" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C43" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C43" s="7" t="s">
-        <v>90</v>
-      </c>
       <c r="D43" s="2" t="s">
         <v>44</v>
       </c>
       <c r="E43" s="7" t="n">
-        <v>-99</v>
+        <v>0</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>43</v>
@@ -2368,16 +2611,16 @@
         <v>43</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E44" s="7" t="n">
-        <v>-99</v>
+        <v>-5</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>44</v>
@@ -2403,16 +2646,16 @@
         <v>44</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>44</v>
       </c>
       <c r="E45" s="7" t="n">
-        <v>-99</v>
+        <v>-10</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>43</v>
@@ -2438,16 +2681,16 @@
         <v>45</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E46" s="7" t="n">
-        <v>-99</v>
+        <v>-15</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>44</v>
@@ -2473,16 +2716,16 @@
         <v>46</v>
       </c>
       <c r="B47" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C47" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="C47" s="7" t="s">
-        <v>95</v>
-      </c>
       <c r="D47" s="2" t="s">
         <v>44</v>
       </c>
       <c r="E47" s="7" t="n">
-        <v>-99</v>
+        <v>-20</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>43</v>
@@ -2508,16 +2751,16 @@
         <v>47</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E48" s="7" t="n">
-        <v>-99</v>
+        <v>-25</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>44</v>
@@ -2543,16 +2786,16 @@
         <v>48</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>44</v>
       </c>
       <c r="E49" s="7" t="n">
-        <v>-99</v>
+        <v>-30</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>43</v>
@@ -2577,8 +2820,8 @@
       <c r="A50" s="2" t="n">
         <v>49</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>58</v>
+      <c r="B50" s="6" t="s">
+        <v>100</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>59</v>
@@ -2587,7 +2830,7 @@
         <v>43</v>
       </c>
       <c r="E50" s="7" t="n">
-        <v>-99</v>
+        <v>-35</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>44</v>
@@ -2606,8 +2849,8 @@
       <c r="A51" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>58</v>
+      <c r="B51" s="6" t="s">
+        <v>101</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>59</v>
@@ -2616,7 +2859,7 @@
         <v>44</v>
       </c>
       <c r="E51" s="7" t="n">
-        <v>-99</v>
+        <v>-40</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>43</v>
@@ -2635,8 +2878,8 @@
       <c r="A52" s="2" t="n">
         <v>51</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>58</v>
+      <c r="B52" s="6" t="s">
+        <v>102</v>
       </c>
       <c r="C52" s="7" t="s">
         <v>59</v>
@@ -2645,7 +2888,7 @@
         <v>43</v>
       </c>
       <c r="E52" s="7" t="n">
-        <v>-99</v>
+        <v>-45</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>44</v>
@@ -2664,8 +2907,8 @@
       <c r="A53" s="2" t="n">
         <v>52</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>58</v>
+      <c r="B53" s="6" t="s">
+        <v>103</v>
       </c>
       <c r="C53" s="7" t="s">
         <v>59</v>
@@ -2693,8 +2936,8 @@
       <c r="A54" s="2" t="n">
         <v>53</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>58</v>
+      <c r="B54" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>59</v>
@@ -2703,7 +2946,7 @@
         <v>43</v>
       </c>
       <c r="E54" s="7" t="n">
-        <v>-99</v>
+        <v>10</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>44</v>
@@ -2722,8 +2965,8 @@
       <c r="A55" s="2" t="n">
         <v>54</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>58</v>
+      <c r="B55" s="6" t="s">
+        <v>105</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>59</v>
@@ -2732,7 +2975,7 @@
         <v>44</v>
       </c>
       <c r="E55" s="7" t="n">
-        <v>-99</v>
+        <v>5</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>43</v>
@@ -2751,8 +2994,8 @@
       <c r="A56" s="2" t="n">
         <v>55</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>58</v>
+      <c r="B56" s="6" t="s">
+        <v>106</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>59</v>
@@ -2761,7 +3004,7 @@
         <v>43</v>
       </c>
       <c r="E56" s="7" t="n">
-        <v>-99</v>
+        <v>0</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>44</v>
@@ -2780,8 +3023,8 @@
       <c r="A57" s="2" t="n">
         <v>56</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>58</v>
+      <c r="B57" s="6" t="s">
+        <v>107</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>59</v>
@@ -2790,7 +3033,7 @@
         <v>44</v>
       </c>
       <c r="E57" s="7" t="n">
-        <v>-99</v>
+        <v>-5</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>43</v>
@@ -2809,8 +3052,8 @@
       <c r="A58" s="2" t="n">
         <v>57</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>58</v>
+      <c r="B58" s="6" t="s">
+        <v>108</v>
       </c>
       <c r="C58" s="7" t="s">
         <v>59</v>
@@ -2819,7 +3062,7 @@
         <v>43</v>
       </c>
       <c r="E58" s="7" t="n">
-        <v>-99</v>
+        <v>-10</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>44</v>
@@ -2838,8 +3081,8 @@
       <c r="A59" s="2" t="n">
         <v>58</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>58</v>
+      <c r="B59" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="C59" s="7" t="s">
         <v>59</v>
@@ -2848,7 +3091,7 @@
         <v>44</v>
       </c>
       <c r="E59" s="7" t="n">
-        <v>-99</v>
+        <v>-15</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>43</v>
@@ -2867,8 +3110,8 @@
       <c r="A60" s="2" t="n">
         <v>59</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>58</v>
+      <c r="B60" s="6" t="s">
+        <v>110</v>
       </c>
       <c r="C60" s="7" t="s">
         <v>59</v>
@@ -2877,7 +3120,7 @@
         <v>43</v>
       </c>
       <c r="E60" s="7" t="n">
-        <v>-99</v>
+        <v>-20</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>44</v>
@@ -2896,8 +3139,8 @@
       <c r="A61" s="2" t="n">
         <v>60</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>58</v>
+      <c r="B61" s="6" t="s">
+        <v>111</v>
       </c>
       <c r="C61" s="7" t="s">
         <v>59</v>
@@ -2906,7 +3149,7 @@
         <v>44</v>
       </c>
       <c r="E61" s="7" t="n">
-        <v>-99</v>
+        <v>-25</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>43</v>
@@ -2925,8 +3168,8 @@
       <c r="A62" s="2" t="n">
         <v>61</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>58</v>
+      <c r="B62" s="6" t="s">
+        <v>112</v>
       </c>
       <c r="C62" s="7" t="s">
         <v>59</v>
@@ -2935,7 +3178,7 @@
         <v>43</v>
       </c>
       <c r="E62" s="7" t="n">
-        <v>-99</v>
+        <v>-30</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>44</v>
@@ -2954,8 +3197,8 @@
       <c r="A63" s="2" t="n">
         <v>62</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>58</v>
+      <c r="B63" s="6" t="s">
+        <v>113</v>
       </c>
       <c r="C63" s="7" t="s">
         <v>59</v>
@@ -2964,7 +3207,7 @@
         <v>44</v>
       </c>
       <c r="E63" s="7" t="n">
-        <v>-99</v>
+        <v>-35</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>43</v>
@@ -2983,8 +3226,8 @@
       <c r="A64" s="2" t="n">
         <v>63</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>58</v>
+      <c r="B64" s="6" t="s">
+        <v>114</v>
       </c>
       <c r="C64" s="7" t="s">
         <v>59</v>
@@ -2993,7 +3236,7 @@
         <v>43</v>
       </c>
       <c r="E64" s="7" t="n">
-        <v>-99</v>
+        <v>-40</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>44</v>
@@ -3012,8 +3255,8 @@
       <c r="A65" s="2" t="n">
         <v>64</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>58</v>
+      <c r="B65" s="6" t="s">
+        <v>115</v>
       </c>
       <c r="C65" s="7" t="s">
         <v>59</v>
@@ -3022,7 +3265,7 @@
         <v>44</v>
       </c>
       <c r="E65" s="7" t="n">
-        <v>-99</v>
+        <v>-45</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>43</v>
@@ -3041,8 +3284,8 @@
       <c r="A66" s="2" t="n">
         <v>65</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>58</v>
+      <c r="B66" s="6" t="s">
+        <v>116</v>
       </c>
       <c r="C66" s="7" t="s">
         <v>59</v>
@@ -3070,8 +3313,8 @@
       <c r="A67" s="2" t="n">
         <v>66</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>58</v>
+      <c r="B67" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="C67" s="7" t="s">
         <v>59</v>
@@ -3080,7 +3323,7 @@
         <v>44</v>
       </c>
       <c r="E67" s="7" t="n">
-        <v>-99</v>
+        <v>10</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>43</v>
@@ -3099,8 +3342,8 @@
       <c r="A68" s="2" t="n">
         <v>67</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>58</v>
+      <c r="B68" s="6" t="s">
+        <v>118</v>
       </c>
       <c r="C68" s="7" t="s">
         <v>59</v>
@@ -3109,7 +3352,7 @@
         <v>43</v>
       </c>
       <c r="E68" s="7" t="n">
-        <v>-99</v>
+        <v>5</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>44</v>
@@ -3128,8 +3371,8 @@
       <c r="A69" s="2" t="n">
         <v>68</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>58</v>
+      <c r="B69" s="6" t="s">
+        <v>119</v>
       </c>
       <c r="C69" s="7" t="s">
         <v>59</v>
@@ -3138,7 +3381,7 @@
         <v>44</v>
       </c>
       <c r="E69" s="7" t="n">
-        <v>-99</v>
+        <v>0</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>43</v>
@@ -3157,8 +3400,8 @@
       <c r="A70" s="2" t="n">
         <v>69</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>58</v>
+      <c r="B70" s="6" t="s">
+        <v>120</v>
       </c>
       <c r="C70" s="7" t="s">
         <v>59</v>
@@ -3167,7 +3410,7 @@
         <v>43</v>
       </c>
       <c r="E70" s="7" t="n">
-        <v>-99</v>
+        <v>-5</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>44</v>
@@ -3186,8 +3429,8 @@
       <c r="A71" s="2" t="n">
         <v>70</v>
       </c>
-      <c r="B71" s="1" t="s">
-        <v>58</v>
+      <c r="B71" s="6" t="s">
+        <v>121</v>
       </c>
       <c r="C71" s="7" t="s">
         <v>59</v>
@@ -3196,7 +3439,7 @@
         <v>44</v>
       </c>
       <c r="E71" s="7" t="n">
-        <v>-99</v>
+        <v>-10</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>43</v>
@@ -3215,8 +3458,8 @@
       <c r="A72" s="2" t="n">
         <v>71</v>
       </c>
-      <c r="B72" s="1" t="s">
-        <v>58</v>
+      <c r="B72" s="6" t="s">
+        <v>122</v>
       </c>
       <c r="C72" s="7" t="s">
         <v>59</v>
@@ -3225,7 +3468,7 @@
         <v>43</v>
       </c>
       <c r="E72" s="7" t="n">
-        <v>-99</v>
+        <v>-15</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>44</v>
@@ -3244,8 +3487,8 @@
       <c r="A73" s="2" t="n">
         <v>72</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>58</v>
+      <c r="B73" s="6" t="s">
+        <v>123</v>
       </c>
       <c r="C73" s="7" t="s">
         <v>59</v>
@@ -3254,7 +3497,7 @@
         <v>44</v>
       </c>
       <c r="E73" s="7" t="n">
-        <v>-99</v>
+        <v>-20</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>43</v>
@@ -3273,8 +3516,8 @@
       <c r="A74" s="2" t="n">
         <v>73</v>
       </c>
-      <c r="B74" s="1" t="s">
-        <v>58</v>
+      <c r="B74" s="6" t="s">
+        <v>124</v>
       </c>
       <c r="C74" s="7" t="s">
         <v>59</v>
@@ -3283,7 +3526,7 @@
         <v>43</v>
       </c>
       <c r="E74" s="7" t="n">
-        <v>-99</v>
+        <v>-25</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>44</v>
@@ -3302,8 +3545,8 @@
       <c r="A75" s="2" t="n">
         <v>74</v>
       </c>
-      <c r="B75" s="1" t="s">
-        <v>58</v>
+      <c r="B75" s="6" t="s">
+        <v>125</v>
       </c>
       <c r="C75" s="7" t="s">
         <v>59</v>
@@ -3312,7 +3555,7 @@
         <v>44</v>
       </c>
       <c r="E75" s="7" t="n">
-        <v>-99</v>
+        <v>-30</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>43</v>
@@ -3331,8 +3574,8 @@
       <c r="A76" s="2" t="n">
         <v>75</v>
       </c>
-      <c r="B76" s="1" t="s">
-        <v>58</v>
+      <c r="B76" s="6" t="s">
+        <v>126</v>
       </c>
       <c r="C76" s="7" t="s">
         <v>59</v>
@@ -3341,7 +3584,7 @@
         <v>43</v>
       </c>
       <c r="E76" s="7" t="n">
-        <v>-99</v>
+        <v>-35</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>44</v>
@@ -3360,8 +3603,8 @@
       <c r="A77" s="2" t="n">
         <v>76</v>
       </c>
-      <c r="B77" s="1" t="s">
-        <v>58</v>
+      <c r="B77" s="6" t="s">
+        <v>127</v>
       </c>
       <c r="C77" s="7" t="s">
         <v>59</v>
@@ -3370,7 +3613,7 @@
         <v>44</v>
       </c>
       <c r="E77" s="7" t="n">
-        <v>-99</v>
+        <v>-40</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>43</v>
@@ -3389,8 +3632,8 @@
       <c r="A78" s="2" t="n">
         <v>77</v>
       </c>
-      <c r="B78" s="1" t="s">
-        <v>58</v>
+      <c r="B78" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C78" s="7" t="s">
         <v>59</v>
@@ -3399,7 +3642,7 @@
         <v>43</v>
       </c>
       <c r="E78" s="7" t="n">
-        <v>-99</v>
+        <v>-45</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>44</v>
@@ -3418,8 +3661,8 @@
       <c r="A79" s="2" t="n">
         <v>78</v>
       </c>
-      <c r="B79" s="1" t="s">
-        <v>58</v>
+      <c r="B79" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="C79" s="7" t="s">
         <v>59</v>
@@ -3447,8 +3690,8 @@
       <c r="A80" s="2" t="n">
         <v>79</v>
       </c>
-      <c r="B80" s="1" t="s">
-        <v>58</v>
+      <c r="B80" s="6" t="s">
+        <v>130</v>
       </c>
       <c r="C80" s="7" t="s">
         <v>59</v>
@@ -3457,7 +3700,7 @@
         <v>43</v>
       </c>
       <c r="E80" s="7" t="n">
-        <v>-99</v>
+        <v>10</v>
       </c>
       <c r="F80" s="2" t="s">
         <v>44</v>
@@ -3476,8 +3719,8 @@
       <c r="A81" s="2" t="n">
         <v>80</v>
       </c>
-      <c r="B81" s="1" t="s">
-        <v>58</v>
+      <c r="B81" s="6" t="s">
+        <v>131</v>
       </c>
       <c r="C81" s="7" t="s">
         <v>59</v>
@@ -3486,7 +3729,7 @@
         <v>44</v>
       </c>
       <c r="E81" s="7" t="n">
-        <v>-99</v>
+        <v>5</v>
       </c>
       <c r="F81" s="2" t="s">
         <v>43</v>
@@ -3505,8 +3748,8 @@
       <c r="A82" s="2" t="n">
         <v>81</v>
       </c>
-      <c r="B82" s="1" t="s">
-        <v>58</v>
+      <c r="B82" s="6" t="s">
+        <v>132</v>
       </c>
       <c r="C82" s="7" t="s">
         <v>59</v>
@@ -3515,7 +3758,7 @@
         <v>43</v>
       </c>
       <c r="E82" s="7" t="n">
-        <v>-99</v>
+        <v>0</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>44</v>
@@ -3534,8 +3777,8 @@
       <c r="A83" s="2" t="n">
         <v>82</v>
       </c>
-      <c r="B83" s="1" t="s">
-        <v>58</v>
+      <c r="B83" s="6" t="s">
+        <v>133</v>
       </c>
       <c r="C83" s="7" t="s">
         <v>59</v>
@@ -3544,7 +3787,7 @@
         <v>44</v>
       </c>
       <c r="E83" s="7" t="n">
-        <v>-99</v>
+        <v>-5</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>43</v>
@@ -3563,8 +3806,8 @@
       <c r="A84" s="2" t="n">
         <v>83</v>
       </c>
-      <c r="B84" s="1" t="s">
-        <v>58</v>
+      <c r="B84" s="6" t="s">
+        <v>134</v>
       </c>
       <c r="C84" s="7" t="s">
         <v>59</v>
@@ -3573,7 +3816,7 @@
         <v>43</v>
       </c>
       <c r="E84" s="7" t="n">
-        <v>-99</v>
+        <v>-10</v>
       </c>
       <c r="F84" s="2" t="s">
         <v>44</v>
@@ -3592,8 +3835,8 @@
       <c r="A85" s="2" t="n">
         <v>84</v>
       </c>
-      <c r="B85" s="1" t="s">
-        <v>58</v>
+      <c r="B85" s="6" t="s">
+        <v>135</v>
       </c>
       <c r="C85" s="7" t="s">
         <v>59</v>
@@ -3602,7 +3845,7 @@
         <v>44</v>
       </c>
       <c r="E85" s="7" t="n">
-        <v>-99</v>
+        <v>-15</v>
       </c>
       <c r="F85" s="2" t="s">
         <v>43</v>
@@ -3621,8 +3864,8 @@
       <c r="A86" s="2" t="n">
         <v>85</v>
       </c>
-      <c r="B86" s="1" t="s">
-        <v>58</v>
+      <c r="B86" s="6" t="s">
+        <v>136</v>
       </c>
       <c r="C86" s="7" t="s">
         <v>59</v>
@@ -3631,7 +3874,7 @@
         <v>43</v>
       </c>
       <c r="E86" s="7" t="n">
-        <v>-99</v>
+        <v>-20</v>
       </c>
       <c r="F86" s="2" t="s">
         <v>44</v>
@@ -3650,8 +3893,8 @@
       <c r="A87" s="2" t="n">
         <v>86</v>
       </c>
-      <c r="B87" s="1" t="s">
-        <v>58</v>
+      <c r="B87" s="6" t="s">
+        <v>137</v>
       </c>
       <c r="C87" s="7" t="s">
         <v>59</v>
@@ -3660,7 +3903,7 @@
         <v>44</v>
       </c>
       <c r="E87" s="7" t="n">
-        <v>-99</v>
+        <v>-25</v>
       </c>
       <c r="F87" s="2" t="s">
         <v>43</v>
@@ -3679,8 +3922,8 @@
       <c r="A88" s="2" t="n">
         <v>87</v>
       </c>
-      <c r="B88" s="1" t="s">
-        <v>58</v>
+      <c r="B88" s="6" t="s">
+        <v>138</v>
       </c>
       <c r="C88" s="7" t="s">
         <v>59</v>
@@ -3689,7 +3932,7 @@
         <v>43</v>
       </c>
       <c r="E88" s="7" t="n">
-        <v>-99</v>
+        <v>-30</v>
       </c>
       <c r="F88" s="2" t="s">
         <v>44</v>
@@ -3708,8 +3951,8 @@
       <c r="A89" s="2" t="n">
         <v>88</v>
       </c>
-      <c r="B89" s="1" t="s">
-        <v>58</v>
+      <c r="B89" s="6" t="s">
+        <v>139</v>
       </c>
       <c r="C89" s="7" t="s">
         <v>59</v>
@@ -3718,7 +3961,7 @@
         <v>44</v>
       </c>
       <c r="E89" s="7" t="n">
-        <v>-99</v>
+        <v>-35</v>
       </c>
       <c r="F89" s="2" t="s">
         <v>43</v>
@@ -3737,8 +3980,8 @@
       <c r="A90" s="2" t="n">
         <v>89</v>
       </c>
-      <c r="B90" s="1" t="s">
-        <v>58</v>
+      <c r="B90" s="6" t="s">
+        <v>140</v>
       </c>
       <c r="C90" s="7" t="s">
         <v>59</v>
@@ -3747,7 +3990,7 @@
         <v>43</v>
       </c>
       <c r="E90" s="7" t="n">
-        <v>-99</v>
+        <v>-40</v>
       </c>
       <c r="F90" s="2" t="s">
         <v>44</v>
@@ -3766,8 +4009,8 @@
       <c r="A91" s="2" t="n">
         <v>90</v>
       </c>
-      <c r="B91" s="1" t="s">
-        <v>58</v>
+      <c r="B91" s="6" t="s">
+        <v>141</v>
       </c>
       <c r="C91" s="7" t="s">
         <v>59</v>
@@ -3776,7 +4019,7 @@
         <v>44</v>
       </c>
       <c r="E91" s="7" t="n">
-        <v>-99</v>
+        <v>-45</v>
       </c>
       <c r="F91" s="2" t="s">
         <v>43</v>
@@ -3795,8 +4038,8 @@
       <c r="A92" s="2" t="n">
         <v>91</v>
       </c>
-      <c r="B92" s="1" t="s">
-        <v>58</v>
+      <c r="B92" s="6" t="s">
+        <v>142</v>
       </c>
       <c r="C92" s="7" t="s">
         <v>59</v>
@@ -3824,8 +4067,8 @@
       <c r="A93" s="2" t="n">
         <v>92</v>
       </c>
-      <c r="B93" s="1" t="s">
-        <v>58</v>
+      <c r="B93" s="6" t="s">
+        <v>143</v>
       </c>
       <c r="C93" s="7" t="s">
         <v>59</v>
@@ -3834,7 +4077,7 @@
         <v>44</v>
       </c>
       <c r="E93" s="7" t="n">
-        <v>-99</v>
+        <v>10</v>
       </c>
       <c r="F93" s="2" t="s">
         <v>43</v>
@@ -3853,8 +4096,8 @@
       <c r="A94" s="2" t="n">
         <v>93</v>
       </c>
-      <c r="B94" s="1" t="s">
-        <v>58</v>
+      <c r="B94" s="6" t="s">
+        <v>144</v>
       </c>
       <c r="C94" s="7" t="s">
         <v>59</v>
@@ -3863,7 +4106,7 @@
         <v>43</v>
       </c>
       <c r="E94" s="7" t="n">
-        <v>-99</v>
+        <v>5</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>44</v>
@@ -3882,8 +4125,8 @@
       <c r="A95" s="2" t="n">
         <v>94</v>
       </c>
-      <c r="B95" s="1" t="s">
-        <v>58</v>
+      <c r="B95" s="6" t="s">
+        <v>145</v>
       </c>
       <c r="C95" s="7" t="s">
         <v>59</v>
@@ -3892,7 +4135,7 @@
         <v>44</v>
       </c>
       <c r="E95" s="7" t="n">
-        <v>-99</v>
+        <v>0</v>
       </c>
       <c r="F95" s="2" t="s">
         <v>43</v>
@@ -3911,8 +4154,8 @@
       <c r="A96" s="2" t="n">
         <v>95</v>
       </c>
-      <c r="B96" s="1" t="s">
-        <v>58</v>
+      <c r="B96" s="6" t="s">
+        <v>146</v>
       </c>
       <c r="C96" s="7" t="s">
         <v>59</v>
@@ -3921,7 +4164,7 @@
         <v>43</v>
       </c>
       <c r="E96" s="7" t="n">
-        <v>-99</v>
+        <v>-5</v>
       </c>
       <c r="F96" s="2" t="s">
         <v>44</v>
@@ -3940,8 +4183,8 @@
       <c r="A97" s="2" t="n">
         <v>96</v>
       </c>
-      <c r="B97" s="1" t="s">
-        <v>58</v>
+      <c r="B97" s="6" t="s">
+        <v>147</v>
       </c>
       <c r="C97" s="7" t="s">
         <v>59</v>
@@ -3950,7 +4193,7 @@
         <v>44</v>
       </c>
       <c r="E97" s="7" t="n">
-        <v>-99</v>
+        <v>-10</v>
       </c>
       <c r="F97" s="2" t="s">
         <v>43</v>
@@ -3969,8 +4212,8 @@
       <c r="A98" s="2" t="n">
         <v>97</v>
       </c>
-      <c r="B98" s="1" t="s">
-        <v>58</v>
+      <c r="B98" s="6" t="s">
+        <v>148</v>
       </c>
       <c r="C98" s="7" t="s">
         <v>59</v>
@@ -3979,7 +4222,7 @@
         <v>43</v>
       </c>
       <c r="E98" s="7" t="n">
-        <v>-99</v>
+        <v>-15</v>
       </c>
       <c r="F98" s="2" t="s">
         <v>44</v>
@@ -3998,8 +4241,8 @@
       <c r="A99" s="2" t="n">
         <v>98</v>
       </c>
-      <c r="B99" s="1" t="s">
-        <v>58</v>
+      <c r="B99" s="6" t="s">
+        <v>149</v>
       </c>
       <c r="C99" s="7" t="s">
         <v>59</v>
@@ -4008,7 +4251,7 @@
         <v>44</v>
       </c>
       <c r="E99" s="7" t="n">
-        <v>-99</v>
+        <v>-20</v>
       </c>
       <c r="F99" s="2" t="s">
         <v>43</v>
@@ -4027,8 +4270,8 @@
       <c r="A100" s="2" t="n">
         <v>99</v>
       </c>
-      <c r="B100" s="1" t="s">
-        <v>58</v>
+      <c r="B100" s="6" t="s">
+        <v>150</v>
       </c>
       <c r="C100" s="7" t="s">
         <v>59</v>
@@ -4037,7 +4280,7 @@
         <v>43</v>
       </c>
       <c r="E100" s="7" t="n">
-        <v>-99</v>
+        <v>-25</v>
       </c>
       <c r="F100" s="2" t="s">
         <v>44</v>
@@ -4056,8 +4299,8 @@
       <c r="A101" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="B101" s="1" t="s">
-        <v>58</v>
+      <c r="B101" s="6" t="s">
+        <v>151</v>
       </c>
       <c r="C101" s="7" t="s">
         <v>59</v>
@@ -4066,7 +4309,7 @@
         <v>44</v>
       </c>
       <c r="E101" s="7" t="n">
-        <v>-99</v>
+        <v>-30</v>
       </c>
       <c r="F101" s="2" t="s">
         <v>43</v>
@@ -4085,8 +4328,8 @@
       <c r="A102" s="2" t="n">
         <v>101</v>
       </c>
-      <c r="B102" s="1" t="s">
-        <v>58</v>
+      <c r="B102" s="6" t="s">
+        <v>152</v>
       </c>
       <c r="C102" s="7" t="s">
         <v>59</v>
@@ -4095,7 +4338,7 @@
         <v>43</v>
       </c>
       <c r="E102" s="7" t="n">
-        <v>-99</v>
+        <v>-35</v>
       </c>
       <c r="F102" s="2" t="s">
         <v>44</v>
@@ -4114,8 +4357,8 @@
       <c r="A103" s="2" t="n">
         <v>102</v>
       </c>
-      <c r="B103" s="1" t="s">
-        <v>58</v>
+      <c r="B103" s="6" t="s">
+        <v>153</v>
       </c>
       <c r="C103" s="7" t="s">
         <v>59</v>
@@ -4124,7 +4367,7 @@
         <v>44</v>
       </c>
       <c r="E103" s="7" t="n">
-        <v>-99</v>
+        <v>-40</v>
       </c>
       <c r="F103" s="2" t="s">
         <v>43</v>
@@ -4143,8 +4386,8 @@
       <c r="A104" s="2" t="n">
         <v>103</v>
       </c>
-      <c r="B104" s="1" t="s">
-        <v>58</v>
+      <c r="B104" s="6" t="s">
+        <v>154</v>
       </c>
       <c r="C104" s="7" t="s">
         <v>59</v>
@@ -4153,7 +4396,7 @@
         <v>43</v>
       </c>
       <c r="E104" s="7" t="n">
-        <v>-99</v>
+        <v>-45</v>
       </c>
       <c r="F104" s="2" t="s">
         <v>44</v>
@@ -4172,8 +4415,8 @@
       <c r="A105" s="2" t="n">
         <v>104</v>
       </c>
-      <c r="B105" s="1" t="s">
-        <v>58</v>
+      <c r="B105" s="6" t="s">
+        <v>155</v>
       </c>
       <c r="C105" s="7" t="s">
         <v>59</v>
@@ -4201,8 +4444,8 @@
       <c r="A106" s="2" t="n">
         <v>105</v>
       </c>
-      <c r="B106" s="1" t="s">
-        <v>58</v>
+      <c r="B106" s="6" t="s">
+        <v>156</v>
       </c>
       <c r="C106" s="7" t="s">
         <v>59</v>
@@ -4211,7 +4454,7 @@
         <v>43</v>
       </c>
       <c r="E106" s="7" t="n">
-        <v>-99</v>
+        <v>10</v>
       </c>
       <c r="F106" s="2" t="s">
         <v>44</v>
@@ -4230,8 +4473,8 @@
       <c r="A107" s="2" t="n">
         <v>106</v>
       </c>
-      <c r="B107" s="1" t="s">
-        <v>58</v>
+      <c r="B107" s="6" t="s">
+        <v>157</v>
       </c>
       <c r="C107" s="7" t="s">
         <v>59</v>
@@ -4240,7 +4483,7 @@
         <v>44</v>
       </c>
       <c r="E107" s="7" t="n">
-        <v>-99</v>
+        <v>5</v>
       </c>
       <c r="F107" s="2" t="s">
         <v>43</v>
@@ -4259,8 +4502,8 @@
       <c r="A108" s="2" t="n">
         <v>107</v>
       </c>
-      <c r="B108" s="1" t="s">
-        <v>58</v>
+      <c r="B108" s="6" t="s">
+        <v>158</v>
       </c>
       <c r="C108" s="7" t="s">
         <v>59</v>
@@ -4269,7 +4512,7 @@
         <v>43</v>
       </c>
       <c r="E108" s="7" t="n">
-        <v>-99</v>
+        <v>0</v>
       </c>
       <c r="F108" s="2" t="s">
         <v>44</v>
@@ -4288,8 +4531,8 @@
       <c r="A109" s="2" t="n">
         <v>108</v>
       </c>
-      <c r="B109" s="1" t="s">
-        <v>58</v>
+      <c r="B109" s="6" t="s">
+        <v>159</v>
       </c>
       <c r="C109" s="7" t="s">
         <v>59</v>
@@ -4298,7 +4541,7 @@
         <v>44</v>
       </c>
       <c r="E109" s="7" t="n">
-        <v>-99</v>
+        <v>-5</v>
       </c>
       <c r="F109" s="2" t="s">
         <v>43</v>
@@ -4317,8 +4560,8 @@
       <c r="A110" s="2" t="n">
         <v>109</v>
       </c>
-      <c r="B110" s="1" t="s">
-        <v>58</v>
+      <c r="B110" s="6" t="s">
+        <v>160</v>
       </c>
       <c r="C110" s="7" t="s">
         <v>59</v>
@@ -4327,7 +4570,7 @@
         <v>43</v>
       </c>
       <c r="E110" s="7" t="n">
-        <v>-99</v>
+        <v>-10</v>
       </c>
       <c r="F110" s="2" t="s">
         <v>44</v>
@@ -4346,8 +4589,8 @@
       <c r="A111" s="2" t="n">
         <v>110</v>
       </c>
-      <c r="B111" s="1" t="s">
-        <v>58</v>
+      <c r="B111" s="6" t="s">
+        <v>161</v>
       </c>
       <c r="C111" s="7" t="s">
         <v>59</v>
@@ -4356,7 +4599,7 @@
         <v>44</v>
       </c>
       <c r="E111" s="7" t="n">
-        <v>-99</v>
+        <v>-15</v>
       </c>
       <c r="F111" s="2" t="s">
         <v>43</v>
@@ -4375,8 +4618,8 @@
       <c r="A112" s="2" t="n">
         <v>111</v>
       </c>
-      <c r="B112" s="1" t="s">
-        <v>58</v>
+      <c r="B112" s="6" t="s">
+        <v>162</v>
       </c>
       <c r="C112" s="7" t="s">
         <v>59</v>
@@ -4385,7 +4628,7 @@
         <v>43</v>
       </c>
       <c r="E112" s="7" t="n">
-        <v>-99</v>
+        <v>-20</v>
       </c>
       <c r="F112" s="2" t="s">
         <v>44</v>
@@ -4404,8 +4647,8 @@
       <c r="A113" s="2" t="n">
         <v>112</v>
       </c>
-      <c r="B113" s="1" t="s">
-        <v>58</v>
+      <c r="B113" s="6" t="s">
+        <v>163</v>
       </c>
       <c r="C113" s="7" t="s">
         <v>59</v>
@@ -4414,7 +4657,7 @@
         <v>44</v>
       </c>
       <c r="E113" s="7" t="n">
-        <v>-99</v>
+        <v>-25</v>
       </c>
       <c r="F113" s="2" t="s">
         <v>43</v>
@@ -4433,8 +4676,8 @@
       <c r="A114" s="2" t="n">
         <v>113</v>
       </c>
-      <c r="B114" s="1" t="s">
-        <v>58</v>
+      <c r="B114" s="6" t="s">
+        <v>164</v>
       </c>
       <c r="C114" s="7" t="s">
         <v>59</v>
@@ -4443,7 +4686,7 @@
         <v>43</v>
       </c>
       <c r="E114" s="7" t="n">
-        <v>-99</v>
+        <v>-30</v>
       </c>
       <c r="F114" s="2" t="s">
         <v>44</v>
@@ -4462,8 +4705,8 @@
       <c r="A115" s="2" t="n">
         <v>114</v>
       </c>
-      <c r="B115" s="1" t="s">
-        <v>58</v>
+      <c r="B115" s="6" t="s">
+        <v>165</v>
       </c>
       <c r="C115" s="7" t="s">
         <v>59</v>
@@ -4472,7 +4715,7 @@
         <v>44</v>
       </c>
       <c r="E115" s="7" t="n">
-        <v>-99</v>
+        <v>-35</v>
       </c>
       <c r="F115" s="2" t="s">
         <v>43</v>
@@ -4491,8 +4734,8 @@
       <c r="A116" s="2" t="n">
         <v>115</v>
       </c>
-      <c r="B116" s="1" t="s">
-        <v>58</v>
+      <c r="B116" s="6" t="s">
+        <v>166</v>
       </c>
       <c r="C116" s="7" t="s">
         <v>59</v>
@@ -4501,7 +4744,7 @@
         <v>43</v>
       </c>
       <c r="E116" s="7" t="n">
-        <v>-99</v>
+        <v>-40</v>
       </c>
       <c r="F116" s="2" t="s">
         <v>44</v>
@@ -4520,8 +4763,8 @@
       <c r="A117" s="2" t="n">
         <v>116</v>
       </c>
-      <c r="B117" s="1" t="s">
-        <v>58</v>
+      <c r="B117" s="6" t="s">
+        <v>167</v>
       </c>
       <c r="C117" s="7" t="s">
         <v>59</v>
@@ -4530,7 +4773,7 @@
         <v>44</v>
       </c>
       <c r="E117" s="7" t="n">
-        <v>-99</v>
+        <v>-45</v>
       </c>
       <c r="F117" s="2" t="s">
         <v>43</v>
@@ -4549,8 +4792,8 @@
       <c r="A118" s="2" t="n">
         <v>117</v>
       </c>
-      <c r="B118" s="1" t="s">
-        <v>58</v>
+      <c r="B118" s="6" t="s">
+        <v>168</v>
       </c>
       <c r="C118" s="7" t="s">
         <v>59</v>
@@ -4578,8 +4821,8 @@
       <c r="A119" s="2" t="n">
         <v>118</v>
       </c>
-      <c r="B119" s="1" t="s">
-        <v>58</v>
+      <c r="B119" s="6" t="s">
+        <v>169</v>
       </c>
       <c r="C119" s="7" t="s">
         <v>59</v>
@@ -4588,7 +4831,7 @@
         <v>44</v>
       </c>
       <c r="E119" s="7" t="n">
-        <v>-99</v>
+        <v>10</v>
       </c>
       <c r="F119" s="2" t="s">
         <v>43</v>
@@ -4607,8 +4850,8 @@
       <c r="A120" s="2" t="n">
         <v>119</v>
       </c>
-      <c r="B120" s="1" t="s">
-        <v>58</v>
+      <c r="B120" s="6" t="s">
+        <v>170</v>
       </c>
       <c r="C120" s="7" t="s">
         <v>59</v>
@@ -4617,7 +4860,7 @@
         <v>43</v>
       </c>
       <c r="E120" s="7" t="n">
-        <v>-99</v>
+        <v>5</v>
       </c>
       <c r="F120" s="2" t="s">
         <v>44</v>
@@ -4636,8 +4879,8 @@
       <c r="A121" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="B121" s="1" t="s">
-        <v>58</v>
+      <c r="B121" s="6" t="s">
+        <v>171</v>
       </c>
       <c r="C121" s="7" t="s">
         <v>59</v>
@@ -4646,7 +4889,7 @@
         <v>44</v>
       </c>
       <c r="E121" s="7" t="n">
-        <v>-99</v>
+        <v>0</v>
       </c>
       <c r="F121" s="2" t="s">
         <v>43</v>
@@ -4665,8 +4908,8 @@
       <c r="A122" s="2" t="n">
         <v>121</v>
       </c>
-      <c r="B122" s="1" t="s">
-        <v>58</v>
+      <c r="B122" s="6" t="s">
+        <v>172</v>
       </c>
       <c r="C122" s="7" t="s">
         <v>59</v>
@@ -4675,7 +4918,7 @@
         <v>43</v>
       </c>
       <c r="E122" s="7" t="n">
-        <v>-99</v>
+        <v>-5</v>
       </c>
       <c r="F122" s="2" t="s">
         <v>44</v>
@@ -4694,8 +4937,8 @@
       <c r="A123" s="2" t="n">
         <v>122</v>
       </c>
-      <c r="B123" s="1" t="s">
-        <v>58</v>
+      <c r="B123" s="6" t="s">
+        <v>173</v>
       </c>
       <c r="C123" s="7" t="s">
         <v>59</v>
@@ -4704,7 +4947,7 @@
         <v>44</v>
       </c>
       <c r="E123" s="7" t="n">
-        <v>-99</v>
+        <v>-10</v>
       </c>
       <c r="F123" s="2" t="s">
         <v>43</v>
@@ -4723,8 +4966,8 @@
       <c r="A124" s="2" t="n">
         <v>123</v>
       </c>
-      <c r="B124" s="1" t="s">
-        <v>58</v>
+      <c r="B124" s="6" t="s">
+        <v>174</v>
       </c>
       <c r="C124" s="7" t="s">
         <v>59</v>
@@ -4733,7 +4976,7 @@
         <v>43</v>
       </c>
       <c r="E124" s="7" t="n">
-        <v>-99</v>
+        <v>-15</v>
       </c>
       <c r="F124" s="2" t="s">
         <v>44</v>
@@ -4752,8 +4995,8 @@
       <c r="A125" s="2" t="n">
         <v>124</v>
       </c>
-      <c r="B125" s="1" t="s">
-        <v>58</v>
+      <c r="B125" s="6" t="s">
+        <v>175</v>
       </c>
       <c r="C125" s="7" t="s">
         <v>59</v>
@@ -4762,7 +5005,7 @@
         <v>44</v>
       </c>
       <c r="E125" s="7" t="n">
-        <v>-99</v>
+        <v>-20</v>
       </c>
       <c r="F125" s="2" t="s">
         <v>43</v>
@@ -4781,8 +5024,8 @@
       <c r="A126" s="2" t="n">
         <v>125</v>
       </c>
-      <c r="B126" s="1" t="s">
-        <v>58</v>
+      <c r="B126" s="6" t="s">
+        <v>176</v>
       </c>
       <c r="C126" s="7" t="s">
         <v>59</v>
@@ -4791,7 +5034,7 @@
         <v>43</v>
       </c>
       <c r="E126" s="7" t="n">
-        <v>-99</v>
+        <v>-25</v>
       </c>
       <c r="F126" s="2" t="s">
         <v>44</v>
@@ -4810,8 +5053,8 @@
       <c r="A127" s="2" t="n">
         <v>126</v>
       </c>
-      <c r="B127" s="1" t="s">
-        <v>58</v>
+      <c r="B127" s="6" t="s">
+        <v>177</v>
       </c>
       <c r="C127" s="7" t="s">
         <v>59</v>
@@ -4820,7 +5063,7 @@
         <v>44</v>
       </c>
       <c r="E127" s="7" t="n">
-        <v>-99</v>
+        <v>-30</v>
       </c>
       <c r="F127" s="2" t="s">
         <v>43</v>
@@ -4839,8 +5082,8 @@
       <c r="A128" s="2" t="n">
         <v>127</v>
       </c>
-      <c r="B128" s="1" t="s">
-        <v>58</v>
+      <c r="B128" s="6" t="s">
+        <v>178</v>
       </c>
       <c r="C128" s="7" t="s">
         <v>59</v>
@@ -4849,7 +5092,7 @@
         <v>43</v>
       </c>
       <c r="E128" s="7" t="n">
-        <v>-99</v>
+        <v>-35</v>
       </c>
       <c r="F128" s="2" t="s">
         <v>44</v>
@@ -4868,8 +5111,8 @@
       <c r="A129" s="2" t="n">
         <v>128</v>
       </c>
-      <c r="B129" s="1" t="s">
-        <v>58</v>
+      <c r="B129" s="6" t="s">
+        <v>179</v>
       </c>
       <c r="C129" s="7" t="s">
         <v>59</v>
@@ -4878,7 +5121,7 @@
         <v>44</v>
       </c>
       <c r="E129" s="7" t="n">
-        <v>-99</v>
+        <v>-40</v>
       </c>
       <c r="F129" s="2" t="s">
         <v>43</v>
@@ -4925,20 +5168,16 @@
       <formula>"blue"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="4">
+  <dataValidations count="3">
     <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C2:C129" type="list">
       <formula1>"blue,red,yellow,green,light blue,white,purple,black"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E130:E131" type="list">
-      <formula1>"+10,+5,0,-5,-10,-15,-20,-25,-30,-35,-40,-45,-inf"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2:G129" type="decimal">
       <formula1>20</formula1>
       <formula2>2000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E129" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E131" type="list">
       <formula1>"+10,+5,0,-5,-10,-15,-20,-25,-30,-35,-40,-45,-99"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4961,7 +5200,7 @@
   <dimension ref="A1:Q129"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q2" activeCellId="0" sqref="Q2"/>
+      <selection pane="topLeft" activeCell="Q2" activeCellId="1" sqref="E130:E131 Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4978,49 +5217,49 @@
   <sheetData>
     <row r="1" customFormat="false" ht="73.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>99</v>
+        <v>180</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>100</v>
+        <v>181</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>101</v>
+        <v>182</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>102</v>
+        <v>183</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>103</v>
+        <v>184</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="11" t="s">
-        <v>104</v>
+        <v>185</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>105</v>
+        <v>186</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>106</v>
+        <v>187</v>
       </c>
       <c r="J1" s="5"/>
       <c r="K1" s="12" t="s">
-        <v>107</v>
+        <v>188</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>108</v>
+        <v>189</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>109</v>
+        <v>190</v>
       </c>
       <c r="N1" s="5"/>
       <c r="O1" s="13" t="s">
-        <v>110</v>
+        <v>191</v>
       </c>
       <c r="P1" s="13" t="s">
-        <v>111</v>
+        <v>192</v>
       </c>
       <c r="Q1" s="13" t="s">
-        <v>112</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5476,7 +5715,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>113</v>
+        <v>194</v>
       </c>
       <c r="B13" s="2" t="n">
         <v>12</v>
@@ -6299,7 +6538,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>114</v>
+        <v>195</v>
       </c>
       <c r="B33" s="2" t="n">
         <v>32</v>
@@ -6688,7 +6927,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>115</v>
+        <v>196</v>
       </c>
       <c r="B49" s="2" t="n">
         <v>48</v>
@@ -7059,7 +7298,7 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>116</v>
+        <v>197</v>
       </c>
       <c r="B65" s="2" t="n">
         <v>64</v>
@@ -7085,7 +7324,7 @@
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>117</v>
+        <v>198</v>
       </c>
       <c r="B66" s="2" t="n">
         <v>65</v>
@@ -7508,7 +7747,7 @@
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="6" t="s">
-        <v>118</v>
+        <v>199</v>
       </c>
       <c r="B96" s="2" t="n">
         <v>95</v>
@@ -7525,7 +7764,7 @@
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="6" t="s">
-        <v>119</v>
+        <v>200</v>
       </c>
       <c r="B97" s="2" t="n">
         <v>96</v>
@@ -7976,7 +8215,7 @@
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="6" t="s">
-        <v>120</v>
+        <v>201</v>
       </c>
       <c r="B129" s="2" t="n">
         <v>128</v>
@@ -8016,7 +8255,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="E130:E131 B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8028,24 +8267,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>121</v>
+        <v>202</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>122</v>
+        <v>203</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>123</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>124</v>
+        <v>205</v>
       </c>
       <c r="B2" s="7" t="n">
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>125</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
sleeptime a little bit increased testsheet adopted
</commit_message>
<xml_diff>
--- a/dLiveChannelListTesting.xlsx
+++ b/dLiveChannelListTesting.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1524" uniqueCount="207">
   <si>
     <t xml:space="preserve">Channel</t>
   </si>
@@ -198,247 +198,247 @@
     <t xml:space="preserve">TST013</t>
   </si>
   <si>
+    <t xml:space="preserve">red</t>
+  </si>
+  <si>
     <t xml:space="preserve">TST014</t>
   </si>
   <si>
+    <t xml:space="preserve">TST015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">green</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST032</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST036</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST037</t>
+  </si>
+  <si>
+    <t xml:space="preserve">light blue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST038</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST039</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST040</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST041</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST042</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST043</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST044</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST045</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST046</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST047</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST048</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">white</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST051</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST052</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST053</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST054</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST055</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST056</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST057</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST058</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST059</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST060</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST061</t>
+  </si>
+  <si>
+    <t xml:space="preserve">purple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST062</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST063</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST064</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST065</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST066</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST067</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST068</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST069</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST070</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST071</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST072</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST073</t>
+  </si>
+  <si>
     <t xml:space="preserve">black</t>
   </si>
   <si>
-    <t xml:space="preserve">TST015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">red</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST019</t>
+    <t xml:space="preserve">TST074</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST075</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST076</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST077</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST078</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST079</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST080</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST081</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST082</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST083</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST084</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST085</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST086</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TST087</t>
   </si>
   <si>
     <t xml:space="preserve">yellow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">green</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST027</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST028</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST029</t>
-  </si>
-  <si>
-    <t xml:space="preserve">light blue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST030</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST031</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST032</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST033</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST034</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST035</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST036</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST037</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST038</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST039</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST040</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST041</t>
-  </si>
-  <si>
-    <t xml:space="preserve">white</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST042</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST043</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST044</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST045</t>
-  </si>
-  <si>
-    <t xml:space="preserve">purple</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST046</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST047</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST048</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST049</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST050</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST051</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST052</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST053</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST054</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST055</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST056</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST057</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST058</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST059</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST060</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST061</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST062</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST063</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST064</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST065</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST066</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST067</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST068</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST069</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST070</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST071</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST072</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST073</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST074</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST075</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST076</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST077</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST078</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST079</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST080</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST081</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST082</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST083</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST084</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST085</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST086</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST087</t>
   </si>
   <si>
     <t xml:space="preserve">TST088</t>
@@ -943,8 +943,8 @@
   </sheetPr>
   <dimension ref="A1:XFD131"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A114" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E130" activeCellId="0" sqref="E130:E131"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E59" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T71" activeCellId="0" sqref="T71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1573,7 +1573,7 @@
         <v>57</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>43</v>
@@ -1605,10 +1605,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>58</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>59</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>44</v>
@@ -1627,6 +1627,9 @@
       </c>
       <c r="J15" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="AK15" s="2" t="s">
         <v>45</v>
@@ -1640,7 +1643,7 @@
         <v>60</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>43</v>
@@ -1659,6 +1662,9 @@
       </c>
       <c r="J16" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="AK16" s="2" t="s">
         <v>45</v>
@@ -1672,7 +1678,7 @@
         <v>61</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>44</v>
@@ -1691,6 +1697,9 @@
       </c>
       <c r="J17" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="AK17" s="2" t="s">
         <v>45</v>
@@ -1704,7 +1713,7 @@
         <v>62</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>43</v>
@@ -1724,7 +1733,7 @@
       <c r="J18" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="N18" s="2" t="s">
+      <c r="M18" s="2" t="s">
         <v>45</v>
       </c>
       <c r="AK18" s="2" t="s">
@@ -1736,10 +1745,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>44</v>
@@ -1759,7 +1768,7 @@
       <c r="J19" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="N19" s="2" t="s">
+      <c r="M19" s="2" t="s">
         <v>45</v>
       </c>
       <c r="AK19" s="2" t="s">
@@ -1771,10 +1780,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>43</v>
@@ -1794,7 +1803,7 @@
       <c r="J20" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="O20" s="2" t="s">
+      <c r="M20" s="2" t="s">
         <v>45</v>
       </c>
       <c r="AK20" s="2" t="s">
@@ -1806,10 +1815,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>44</v>
@@ -1829,7 +1838,7 @@
       <c r="J21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O21" s="2" t="s">
+      <c r="M21" s="2" t="s">
         <v>45</v>
       </c>
       <c r="AK21" s="2" t="s">
@@ -1841,10 +1850,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>43</v>
@@ -1864,7 +1873,7 @@
       <c r="J22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="O22" s="2" t="s">
+      <c r="M22" s="2" t="s">
         <v>45</v>
       </c>
       <c r="AK22" s="2" t="s">
@@ -1876,10 +1885,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>44</v>
@@ -1899,7 +1908,7 @@
       <c r="J23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O23" s="2" t="s">
+      <c r="M23" s="2" t="s">
         <v>45</v>
       </c>
       <c r="AK23" s="2" t="s">
@@ -1911,10 +1920,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>43</v>
@@ -1934,7 +1943,7 @@
       <c r="J24" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="O24" s="2" t="s">
+      <c r="M24" s="2" t="s">
         <v>45</v>
       </c>
       <c r="AK24" s="2" t="s">
@@ -1946,10 +1955,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>44</v>
@@ -1969,7 +1978,7 @@
       <c r="J25" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O25" s="2" t="s">
+      <c r="M25" s="2" t="s">
         <v>45</v>
       </c>
       <c r="AK25" s="2" t="s">
@@ -1981,10 +1990,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>43</v>
@@ -2004,7 +2013,7 @@
       <c r="J26" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="P26" s="2" t="s">
+      <c r="N26" s="2" t="s">
         <v>45</v>
       </c>
       <c r="AK26" s="2" t="s">
@@ -2016,10 +2025,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>44</v>
@@ -2039,7 +2048,7 @@
       <c r="J27" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="P27" s="2" t="s">
+      <c r="N27" s="2" t="s">
         <v>45</v>
       </c>
       <c r="AK27" s="2" t="s">
@@ -2051,10 +2060,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>43</v>
@@ -2074,7 +2083,7 @@
       <c r="J28" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="P28" s="2" t="s">
+      <c r="N28" s="2" t="s">
         <v>45</v>
       </c>
       <c r="AK28" s="2" t="s">
@@ -2086,10 +2095,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>44</v>
@@ -2109,7 +2118,7 @@
       <c r="J29" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="P29" s="2" t="s">
+      <c r="N29" s="2" t="s">
         <v>45</v>
       </c>
       <c r="AK29" s="2" t="s">
@@ -2121,10 +2130,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>43</v>
@@ -2144,7 +2153,7 @@
       <c r="J30" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="Q30" s="2" t="s">
+      <c r="N30" s="2" t="s">
         <v>45</v>
       </c>
       <c r="AK30" s="2" t="s">
@@ -2156,10 +2165,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>44</v>
@@ -2179,7 +2188,7 @@
       <c r="J31" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="Q31" s="2" t="s">
+      <c r="N31" s="2" t="s">
         <v>45</v>
       </c>
       <c r="AK31" s="2" t="s">
@@ -2191,10 +2200,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>43</v>
@@ -2214,7 +2223,7 @@
       <c r="J32" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="Q32" s="2" t="s">
+      <c r="N32" s="2" t="s">
         <v>45</v>
       </c>
       <c r="AK32" s="2" t="s">
@@ -2226,10 +2235,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>44</v>
@@ -2249,7 +2258,7 @@
       <c r="J33" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="Q33" s="2" t="s">
+      <c r="N33" s="2" t="s">
         <v>45</v>
       </c>
       <c r="AK33" s="2" t="s">
@@ -2261,10 +2270,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>43</v>
@@ -2284,7 +2293,7 @@
       <c r="J34" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="Q34" s="2" t="s">
+      <c r="N34" s="2" t="s">
         <v>45</v>
       </c>
       <c r="AK34" s="2" t="s">
@@ -2296,10 +2305,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>44</v>
@@ -2319,7 +2328,7 @@
       <c r="J35" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="Q35" s="2" t="s">
+      <c r="N35" s="2" t="s">
         <v>45</v>
       </c>
       <c r="AK35" s="2" t="s">
@@ -2331,10 +2340,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>43</v>
@@ -2354,7 +2363,7 @@
       <c r="J36" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="Q36" s="2" t="s">
+      <c r="N36" s="2" t="s">
         <v>45</v>
       </c>
       <c r="AK36" s="2" t="s">
@@ -2366,10 +2375,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>44</v>
@@ -2389,7 +2398,7 @@
       <c r="J37" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="Q37" s="2" t="s">
+      <c r="N37" s="2" t="s">
         <v>45</v>
       </c>
       <c r="AK37" s="2" t="s">
@@ -2401,10 +2410,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>43</v>
@@ -2424,7 +2433,7 @@
       <c r="J38" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="R38" s="2" t="s">
+      <c r="O38" s="2" t="s">
         <v>45</v>
       </c>
       <c r="AK38" s="2" t="s">
@@ -2436,10 +2445,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>44</v>
@@ -2459,7 +2468,7 @@
       <c r="J39" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="R39" s="2" t="s">
+      <c r="O39" s="2" t="s">
         <v>45</v>
       </c>
       <c r="AK39" s="2" t="s">
@@ -2471,10 +2480,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>43</v>
@@ -2494,7 +2503,7 @@
       <c r="J40" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="R40" s="2" t="s">
+      <c r="O40" s="2" t="s">
         <v>45</v>
       </c>
       <c r="AK40" s="2" t="s">
@@ -2506,10 +2515,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>44</v>
@@ -2529,7 +2538,7 @@
       <c r="J41" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="R41" s="2" t="s">
+      <c r="O41" s="2" t="s">
         <v>45</v>
       </c>
       <c r="AK41" s="2" t="s">
@@ -2541,10 +2550,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>43</v>
@@ -2564,7 +2573,7 @@
       <c r="J42" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="S42" s="2" t="s">
+      <c r="O42" s="2" t="s">
         <v>45</v>
       </c>
       <c r="AL42" s="2" t="s">
@@ -2576,10 +2585,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>44</v>
@@ -2599,7 +2608,7 @@
       <c r="J43" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="S43" s="2" t="s">
+      <c r="O43" s="2" t="s">
         <v>45</v>
       </c>
       <c r="AL43" s="2" t="s">
@@ -2611,10 +2620,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>43</v>
@@ -2634,7 +2643,7 @@
       <c r="J44" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="S44" s="2" t="s">
+      <c r="O44" s="2" t="s">
         <v>45</v>
       </c>
       <c r="AL44" s="2" t="s">
@@ -2646,10 +2655,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>44</v>
@@ -2669,7 +2678,7 @@
       <c r="J45" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="S45" s="2" t="s">
+      <c r="O45" s="2" t="s">
         <v>45</v>
       </c>
       <c r="AL45" s="2" t="s">
@@ -2681,10 +2690,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>43</v>
@@ -2704,7 +2713,7 @@
       <c r="J46" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="T46" s="2" t="s">
+      <c r="O46" s="2" t="s">
         <v>45</v>
       </c>
       <c r="AL46" s="2" t="s">
@@ -2716,10 +2725,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>44</v>
@@ -2739,7 +2748,7 @@
       <c r="J47" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="T47" s="2" t="s">
+      <c r="O47" s="2" t="s">
         <v>45</v>
       </c>
       <c r="AL47" s="2" t="s">
@@ -2751,10 +2760,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>43</v>
@@ -2774,7 +2783,7 @@
       <c r="J48" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="T48" s="2" t="s">
+      <c r="O48" s="2" t="s">
         <v>45</v>
       </c>
       <c r="AL48" s="2" t="s">
@@ -2786,10 +2795,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>44</v>
@@ -2809,7 +2818,7 @@
       <c r="J49" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="T49" s="2" t="s">
+      <c r="O49" s="2" t="s">
         <v>45</v>
       </c>
       <c r="AL49" s="2" t="s">
@@ -2821,10 +2830,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>43</v>
@@ -2843,6 +2852,9 @@
       </c>
       <c r="J50" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="P50" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2850,10 +2862,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>44</v>
@@ -2872,6 +2884,9 @@
       </c>
       <c r="J51" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="P51" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2879,10 +2894,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>43</v>
@@ -2901,6 +2916,9 @@
       </c>
       <c r="J52" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="P52" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2908,10 +2926,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>44</v>
@@ -2930,6 +2948,9 @@
       </c>
       <c r="J53" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="P53" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2937,10 +2958,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>43</v>
@@ -2959,6 +2980,9 @@
       </c>
       <c r="J54" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="P54" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2966,10 +2990,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>44</v>
@@ -2988,6 +3012,9 @@
       </c>
       <c r="J55" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="P55" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2995,10 +3022,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>43</v>
@@ -3017,6 +3044,9 @@
       </c>
       <c r="J56" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="P56" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3024,10 +3054,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>44</v>
@@ -3046,6 +3076,9 @@
       </c>
       <c r="J57" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="P57" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3053,10 +3086,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>43</v>
@@ -3075,6 +3108,9 @@
       </c>
       <c r="J58" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="P58" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3082,10 +3118,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>44</v>
@@ -3104,6 +3140,9 @@
       </c>
       <c r="J59" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="P59" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3111,10 +3150,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>43</v>
@@ -3133,6 +3172,9 @@
       </c>
       <c r="J60" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="P60" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3140,10 +3182,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>44</v>
@@ -3162,6 +3204,9 @@
       </c>
       <c r="J61" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="P61" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3169,10 +3214,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>43</v>
@@ -3191,6 +3236,9 @@
       </c>
       <c r="J62" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="Q62" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3198,10 +3246,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>44</v>
@@ -3220,6 +3268,9 @@
       </c>
       <c r="J63" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="Q63" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3227,10 +3278,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>43</v>
@@ -3249,6 +3300,9 @@
       </c>
       <c r="J64" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="Q64" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3256,10 +3310,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>44</v>
@@ -3278,6 +3332,9 @@
       </c>
       <c r="J65" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="Q65" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3285,10 +3342,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>43</v>
@@ -3307,6 +3364,9 @@
       </c>
       <c r="J66" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="Q66" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3314,10 +3374,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>44</v>
@@ -3336,6 +3396,9 @@
       </c>
       <c r="J67" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="Q67" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3343,10 +3406,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>43</v>
@@ -3365,6 +3428,9 @@
       </c>
       <c r="J68" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="Q68" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3372,10 +3438,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>44</v>
@@ -3394,6 +3460,9 @@
       </c>
       <c r="J69" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="Q69" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3401,10 +3470,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>43</v>
@@ -3423,6 +3492,9 @@
       </c>
       <c r="J70" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="Q70" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3430,10 +3502,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>44</v>
@@ -3452,6 +3524,9 @@
       </c>
       <c r="J71" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="Q71" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3459,10 +3534,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>43</v>
@@ -3481,6 +3556,9 @@
       </c>
       <c r="J72" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="Q72" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3488,10 +3566,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>44</v>
@@ -3510,6 +3588,9 @@
       </c>
       <c r="J73" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="Q73" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3517,10 +3598,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>59</v>
+        <v>123</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>43</v>
@@ -3539,6 +3620,9 @@
       </c>
       <c r="J74" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="R74" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3546,10 +3630,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>59</v>
+        <v>123</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>44</v>
@@ -3568,6 +3652,9 @@
       </c>
       <c r="J75" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="R75" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3575,10 +3662,10 @@
         <v>75</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>59</v>
+        <v>123</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>43</v>
@@ -3597,6 +3684,9 @@
       </c>
       <c r="J76" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="R76" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3604,10 +3694,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>59</v>
+        <v>123</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>44</v>
@@ -3626,6 +3716,9 @@
       </c>
       <c r="J77" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="R77" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3633,10 +3726,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>59</v>
+        <v>123</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>43</v>
@@ -3655,6 +3748,9 @@
       </c>
       <c r="J78" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="R78" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3662,10 +3758,10 @@
         <v>78</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>59</v>
+        <v>123</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>44</v>
@@ -3684,6 +3780,9 @@
       </c>
       <c r="J79" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="R79" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3691,10 +3790,10 @@
         <v>79</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>59</v>
+        <v>123</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>43</v>
@@ -3713,6 +3812,9 @@
       </c>
       <c r="J80" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="R80" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3720,10 +3822,10 @@
         <v>80</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>59</v>
+        <v>123</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>44</v>
@@ -3742,6 +3844,9 @@
       </c>
       <c r="J81" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="R81" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3749,10 +3854,10 @@
         <v>81</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>59</v>
+        <v>123</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>43</v>
@@ -3771,6 +3876,9 @@
       </c>
       <c r="J82" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="R82" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3778,10 +3886,10 @@
         <v>82</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>59</v>
+        <v>123</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>44</v>
@@ -3800,6 +3908,9 @@
       </c>
       <c r="J83" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="R83" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3807,10 +3918,10 @@
         <v>83</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>59</v>
+        <v>123</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>43</v>
@@ -3829,6 +3940,9 @@
       </c>
       <c r="J84" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="R84" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3836,10 +3950,10 @@
         <v>84</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>59</v>
+        <v>123</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>44</v>
@@ -3858,6 +3972,9 @@
       </c>
       <c r="J85" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="R85" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3865,10 +3982,10 @@
         <v>85</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>43</v>
@@ -3887,6 +4004,9 @@
       </c>
       <c r="J86" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="S86" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3894,10 +4014,10 @@
         <v>86</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>44</v>
@@ -3916,6 +4036,9 @@
       </c>
       <c r="J87" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="S87" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3923,10 +4046,10 @@
         <v>87</v>
       </c>
       <c r="B88" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C88" s="7" t="s">
         <v>138</v>
-      </c>
-      <c r="C88" s="7" t="s">
-        <v>59</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>43</v>
@@ -3945,6 +4068,9 @@
       </c>
       <c r="J88" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="S88" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3955,7 +4081,7 @@
         <v>139</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>44</v>
@@ -3974,6 +4100,9 @@
       </c>
       <c r="J89" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="S89" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3984,7 +4113,7 @@
         <v>140</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>43</v>
@@ -4003,6 +4132,9 @@
       </c>
       <c r="J90" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="S90" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4013,7 +4145,7 @@
         <v>141</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>44</v>
@@ -4032,6 +4164,9 @@
       </c>
       <c r="J91" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="S91" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4042,7 +4177,7 @@
         <v>142</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>43</v>
@@ -4061,6 +4196,9 @@
       </c>
       <c r="J92" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="S92" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4071,7 +4209,7 @@
         <v>143</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>59</v>
+        <v>123</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>44</v>
@@ -4090,6 +4228,9 @@
       </c>
       <c r="J93" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="S93" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4100,7 +4241,7 @@
         <v>144</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>43</v>
@@ -4119,6 +4260,9 @@
       </c>
       <c r="J94" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="T94" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4129,7 +4273,7 @@
         <v>145</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>44</v>
@@ -4148,6 +4292,9 @@
       </c>
       <c r="J95" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="T95" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4158,7 +4305,7 @@
         <v>146</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>59</v>
+        <v>138</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>43</v>
@@ -4177,6 +4324,9 @@
       </c>
       <c r="J96" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="T96" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4187,7 +4337,7 @@
         <v>147</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>44</v>
@@ -4206,6 +4356,9 @@
       </c>
       <c r="J97" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="T97" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4216,7 +4369,7 @@
         <v>148</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>43</v>
@@ -4235,6 +4388,9 @@
       </c>
       <c r="J98" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="T98" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4245,7 +4401,7 @@
         <v>149</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>44</v>
@@ -4264,6 +4420,9 @@
       </c>
       <c r="J99" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="T99" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4274,7 +4433,7 @@
         <v>150</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>43</v>
@@ -4293,6 +4452,9 @@
       </c>
       <c r="J100" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="T100" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4303,7 +4465,7 @@
         <v>151</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>59</v>
+        <v>123</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>44</v>
@@ -4322,6 +4484,9 @@
       </c>
       <c r="J101" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="T101" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4332,7 +4497,7 @@
         <v>152</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>43</v>
@@ -4351,6 +4516,9 @@
       </c>
       <c r="J102" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="U102" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4361,7 +4529,7 @@
         <v>153</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>44</v>
@@ -4380,6 +4548,9 @@
       </c>
       <c r="J103" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="U103" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4390,7 +4561,7 @@
         <v>154</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>59</v>
+        <v>138</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>43</v>
@@ -4409,6 +4580,9 @@
       </c>
       <c r="J104" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="U104" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4419,7 +4593,7 @@
         <v>155</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>44</v>
@@ -4438,6 +4612,9 @@
       </c>
       <c r="J105" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="U105" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4448,7 +4625,7 @@
         <v>156</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>43</v>
@@ -4467,6 +4644,9 @@
       </c>
       <c r="J106" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="U106" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4477,7 +4657,7 @@
         <v>157</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>44</v>
@@ -4496,6 +4676,9 @@
       </c>
       <c r="J107" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="U107" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4506,7 +4689,7 @@
         <v>158</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>43</v>
@@ -4525,6 +4708,9 @@
       </c>
       <c r="J108" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="U108" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4535,7 +4721,7 @@
         <v>159</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>59</v>
+        <v>123</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>44</v>
@@ -4554,6 +4740,9 @@
       </c>
       <c r="J109" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="U109" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4564,7 +4753,7 @@
         <v>160</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>43</v>
@@ -4583,6 +4772,9 @@
       </c>
       <c r="J110" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="V110" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4593,7 +4785,7 @@
         <v>161</v>
       </c>
       <c r="C111" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>44</v>
@@ -4612,6 +4804,9 @@
       </c>
       <c r="J111" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="V111" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4622,7 +4817,7 @@
         <v>162</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>59</v>
+        <v>138</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>43</v>
@@ -4641,6 +4836,9 @@
       </c>
       <c r="J112" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="V112" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4651,7 +4849,7 @@
         <v>163</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>44</v>
@@ -4670,6 +4868,9 @@
       </c>
       <c r="J113" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="V113" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4680,7 +4881,7 @@
         <v>164</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="D114" s="2" t="s">
         <v>43</v>
@@ -4699,6 +4900,9 @@
       </c>
       <c r="J114" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="V114" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4709,7 +4913,7 @@
         <v>165</v>
       </c>
       <c r="C115" s="7" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="D115" s="2" t="s">
         <v>44</v>
@@ -4728,6 +4932,9 @@
       </c>
       <c r="J115" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="V115" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4738,7 +4945,7 @@
         <v>166</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>43</v>
@@ -4757,6 +4964,9 @@
       </c>
       <c r="J116" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="V116" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4767,7 +4977,7 @@
         <v>167</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>59</v>
+        <v>123</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>44</v>
@@ -4786,6 +4996,9 @@
       </c>
       <c r="J117" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="V117" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4796,7 +5009,7 @@
         <v>168</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="D118" s="2" t="s">
         <v>43</v>
@@ -4815,6 +5028,9 @@
       </c>
       <c r="J118" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="W118" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4825,7 +5041,7 @@
         <v>169</v>
       </c>
       <c r="C119" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>44</v>
@@ -4844,6 +5060,9 @@
       </c>
       <c r="J119" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="W119" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4854,7 +5073,7 @@
         <v>170</v>
       </c>
       <c r="C120" s="7" t="s">
-        <v>59</v>
+        <v>138</v>
       </c>
       <c r="D120" s="2" t="s">
         <v>43</v>
@@ -4873,6 +5092,9 @@
       </c>
       <c r="J120" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="W120" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4883,7 +5105,7 @@
         <v>171</v>
       </c>
       <c r="C121" s="7" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D121" s="2" t="s">
         <v>44</v>
@@ -4902,6 +5124,9 @@
       </c>
       <c r="J121" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="W121" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4912,7 +5137,7 @@
         <v>172</v>
       </c>
       <c r="C122" s="7" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>43</v>
@@ -4931,6 +5156,9 @@
       </c>
       <c r="J122" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="W122" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4941,7 +5169,7 @@
         <v>173</v>
       </c>
       <c r="C123" s="7" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>44</v>
@@ -4960,6 +5188,9 @@
       </c>
       <c r="J123" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="W123" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4970,7 +5201,7 @@
         <v>174</v>
       </c>
       <c r="C124" s="7" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>43</v>
@@ -4989,6 +5220,9 @@
       </c>
       <c r="J124" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="W124" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4999,7 +5233,7 @@
         <v>175</v>
       </c>
       <c r="C125" s="7" t="s">
-        <v>59</v>
+        <v>123</v>
       </c>
       <c r="D125" s="2" t="s">
         <v>44</v>
@@ -5018,6 +5252,9 @@
       </c>
       <c r="J125" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="W125" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5028,7 +5265,7 @@
         <v>176</v>
       </c>
       <c r="C126" s="7" t="s">
-        <v>59</v>
+        <v>123</v>
       </c>
       <c r="D126" s="2" t="s">
         <v>43</v>
@@ -5047,6 +5284,9 @@
       </c>
       <c r="J126" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="X126" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5057,7 +5297,7 @@
         <v>177</v>
       </c>
       <c r="C127" s="7" t="s">
-        <v>59</v>
+        <v>123</v>
       </c>
       <c r="D127" s="2" t="s">
         <v>44</v>
@@ -5076,6 +5316,9 @@
       </c>
       <c r="J127" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="Y127" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5086,7 +5329,7 @@
         <v>178</v>
       </c>
       <c r="C128" s="7" t="s">
-        <v>59</v>
+        <v>123</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>43</v>
@@ -5105,6 +5348,9 @@
       </c>
       <c r="J128" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="Z128" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5115,7 +5361,7 @@
         <v>179</v>
       </c>
       <c r="C129" s="7" t="s">
-        <v>59</v>
+        <v>123</v>
       </c>
       <c r="D129" s="2" t="s">
         <v>44</v>
@@ -5134,6 +5380,9 @@
       </c>
       <c r="J129" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="AA129" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5200,7 +5449,7 @@
   <dimension ref="A1:Q129"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q2" activeCellId="1" sqref="E130:E131 Q2"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5311,7 +5560,7 @@
         <v>44</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E3" s="7" t="n">
         <v>55</v>
@@ -5320,7 +5569,7 @@
         <v>44</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I3" s="7" t="n">
         <v>55</v>
@@ -5329,7 +5578,7 @@
         <v>44</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M3" s="7" t="n">
         <v>55</v>
@@ -5338,7 +5587,7 @@
         <v>44</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q3" s="7" t="n">
         <v>55</v>
@@ -5393,7 +5642,7 @@
         <v>44</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E5" s="7" t="n">
         <v>45</v>
@@ -5402,7 +5651,7 @@
         <v>44</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I5" s="7" t="n">
         <v>45</v>
@@ -5411,7 +5660,7 @@
         <v>44</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M5" s="7" t="n">
         <v>45</v>
@@ -5420,7 +5669,7 @@
         <v>44</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q5" s="7" t="n">
         <v>45</v>
@@ -5475,7 +5724,7 @@
         <v>44</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E7" s="7" t="n">
         <v>35</v>
@@ -5484,7 +5733,7 @@
         <v>44</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I7" s="7" t="n">
         <v>35</v>
@@ -5493,7 +5742,7 @@
         <v>44</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M7" s="7" t="n">
         <v>35</v>
@@ -5502,7 +5751,7 @@
         <v>44</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q7" s="7" t="n">
         <v>35</v>
@@ -5557,7 +5806,7 @@
         <v>44</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E9" s="7" t="n">
         <v>25</v>
@@ -5566,7 +5815,7 @@
         <v>44</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I9" s="7" t="n">
         <v>25</v>
@@ -5575,7 +5824,7 @@
         <v>44</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M9" s="7" t="n">
         <v>25</v>
@@ -5584,7 +5833,7 @@
         <v>44</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q9" s="7" t="n">
         <v>25</v>
@@ -5639,7 +5888,7 @@
         <v>44</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E11" s="7" t="n">
         <v>15</v>
@@ -5648,7 +5897,7 @@
         <v>44</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I11" s="7" t="n">
         <v>15</v>
@@ -5657,7 +5906,7 @@
         <v>44</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M11" s="7" t="n">
         <v>15</v>
@@ -5666,7 +5915,7 @@
         <v>44</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q11" s="7" t="n">
         <v>15</v>
@@ -5724,7 +5973,7 @@
         <v>44</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E13" s="7" t="n">
         <v>5</v>
@@ -5733,7 +5982,7 @@
         <v>44</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I13" s="7" t="n">
         <v>5</v>
@@ -5742,7 +5991,7 @@
         <v>44</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M13" s="7" t="n">
         <v>5</v>
@@ -5751,7 +6000,7 @@
         <v>44</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q13" s="7" t="n">
         <v>5</v>
@@ -8255,7 +8504,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="E130:E131 B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
non group sleeps adjusted readme updated
</commit_message>
<xml_diff>
--- a/dLiveChannelListTesting.xlsx
+++ b/dLiveChannelListTesting.xlsx
@@ -943,8 +943,8 @@
   </sheetPr>
   <dimension ref="A1:XFD131"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A99" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W121" activeCellId="0" sqref="W121"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D97" activeCellId="0" sqref="D97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -968,7 +968,7 @@
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0"/>
+      <c r="C1" s="1"/>
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
@@ -5574,7 +5574,7 @@
       <c r="F131" s="7"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="K1:K1048576 E1:E1048576 D98:D129">
+  <conditionalFormatting sqref="K1:K1048576 E1:E1048576 D2:D129">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"purple"</formula>
     </cfRule>

</xml_diff>